<commit_message>
add IBAN and full Buchung
</commit_message>
<xml_diff>
--- a/pfad-master/pfad-common/src/test/data/ImportPayments.xlsx
+++ b/pfad-master/pfad-common/src/test/data/ImportPayments.xlsx
@@ -22,12 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Gruppenbeitrag 16/17 Name Vorname</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppenbeitrag 16/17 Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gruppenbeitrag 16/17 NameDrei VornameDrei1 VornameDrei2 VornameDrei3</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppenbeitrag 16/17 Corelie Scholz</t>
@@ -146,7 +149,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
@@ -154,12 +157,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.69897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,9 +193,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>42634</v>
+        <v>42636</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>10</v>
@@ -201,12 +204,12 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>42646</v>
+        <v>42634</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>10</v>
@@ -215,10 +218,23 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>42646</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>70</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -368,6 +384,7 @@
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -392,7 +409,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -418,7 +435,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>